<commit_message>
Code added and cleaned up.
</commit_message>
<xml_diff>
--- a/VerificationMatrix.xlsx
+++ b/VerificationMatrix.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\MatlabCode\projects\SingleCellModeling\SingleCellModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FCCA4C-EEBF-44D5-9D4C-EB69144AB24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE450930-2DF5-4EC6-83D2-1D9F0FE74E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="119">
   <si>
     <t>File</t>
   </si>
@@ -75,12 +84,6 @@
     <t>Paths and data fixed.</t>
   </si>
   <si>
-    <t>Where does pseudoBulkModelDataCPM.txt come from, it seems to be used!</t>
-  </si>
-  <si>
-    <t>same with whoever uses pseudoBulkModelDataTMM.txt - find that code</t>
-  </si>
-  <si>
     <t>No specific test cases have been run. The code is fairly simple, just a bunch of figures without any data processing + a straight-forward statistical test in the end.</t>
   </si>
   <si>
@@ -126,12 +129,6 @@
     <t>calcJaccard.m</t>
   </si>
   <si>
-    <t>It comes from GeneratePoolSizeData.m</t>
-  </si>
-  <si>
-    <t>The bulk pool size models are generated by the file generate_PS_models.m, called by cluster scripts</t>
-  </si>
-  <si>
     <t>No specific test cases have been run, however, there are a few small tests embedded in the code. The code mainly calls the functions below, assembles datasets etc.</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>Not specifically tested, the code is fairly trivial.</t>
   </si>
   <si>
-    <t>vänta med dessa, gör ihop med tINIT-tester</t>
-  </si>
-  <si>
     <t>getExprForRxnScore.m</t>
   </si>
   <si>
@@ -154,13 +148,256 @@
   </si>
   <si>
     <t>TC 0104</t>
+  </si>
+  <si>
+    <t>checkTasksExt.m</t>
+  </si>
+  <si>
+    <t>fillGapsOpt.m</t>
+  </si>
+  <si>
+    <t>fitTasksOpt.m</t>
+  </si>
+  <si>
+    <t>getINITModel9.m</t>
+  </si>
+  <si>
+    <t>getMinNrFluxesOpt.m</t>
+  </si>
+  <si>
+    <t>groupRxnScores.m</t>
+  </si>
+  <si>
+    <t>runINIT9.m</t>
+  </si>
+  <si>
+    <t>prepINITModel.m</t>
+  </si>
+  <si>
+    <t>mergeLinear.m</t>
+  </si>
+  <si>
+    <t>rescaleModelForINIT.m</t>
+  </si>
+  <si>
+    <t>reverseRxns.m</t>
+  </si>
+  <si>
+    <t>T0003</t>
+  </si>
+  <si>
+    <t>T0004</t>
+  </si>
+  <si>
+    <t>T0001, T0002, T0050</t>
+  </si>
+  <si>
+    <t>T0001, T0002, T0003, T0050</t>
+  </si>
+  <si>
+    <t>T0001, T0002</t>
+  </si>
+  <si>
+    <t>T0006</t>
+  </si>
+  <si>
+    <t>T0007</t>
+  </si>
+  <si>
+    <t>This is a small change to an existing function in RAVEN. It has not been tested with test cases, although it has been manually tested to produce reasonable results.</t>
+  </si>
+  <si>
+    <t>AnalyzeLC3.m</t>
+  </si>
+  <si>
+    <t>AnalyzeMCOR3.m</t>
+  </si>
+  <si>
+    <t>evaluateEssentialityPredictions.m</t>
+  </si>
+  <si>
+    <t>adjust_pvalues.m</t>
+  </si>
+  <si>
+    <t>enrichment_test.m</t>
+  </si>
+  <si>
+    <t>run_evaless_newalg.sh</t>
+  </si>
+  <si>
+    <t>getTaskEssentialGenes.m</t>
+  </si>
+  <si>
+    <t>run_evaless_oldalg.sh</t>
+  </si>
+  <si>
+    <t>trivial slurm script</t>
+  </si>
+  <si>
+    <t>This code has not been extensively tested - the code is copied from the Human1 paper and slightly modified.</t>
+  </si>
+  <si>
+    <t>Copied from the Human1 paper, untouched.</t>
+  </si>
+  <si>
+    <t>generate_DepMap_models_new_alg.m</t>
+  </si>
+  <si>
+    <t>prepHumanModel.m</t>
+  </si>
+  <si>
+    <t>prepMouseModel.m</t>
+  </si>
+  <si>
+    <t>getAATripletReactions.m</t>
+  </si>
+  <si>
+    <t>removeDrugReactions.m</t>
+  </si>
+  <si>
+    <t>removeUnwantedReactions.m</t>
+  </si>
+  <si>
+    <t>prepDepMapData.m</t>
+  </si>
+  <si>
+    <t>Not tested, fairly trivial code, it just calls the model generation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is not much code. I tested that we keep roughly 65% of the samples after filtering the ones without gene essentiality information, which seems reasonable. </t>
+  </si>
+  <si>
+    <t>The code is fairly simple, not explicitly tested.</t>
+  </si>
+  <si>
+    <t>This code was tested while written, there are a few printouts commented out in the code.</t>
+  </si>
+  <si>
+    <t>The code is trivial and not explicitly tested, although it was tested when written.</t>
+  </si>
+  <si>
+    <t>mergeClusterData.m</t>
+  </si>
+  <si>
+    <t>generate_DepMap_models.m</t>
+  </si>
+  <si>
+    <t>run_gen_depmap_models.sh</t>
+  </si>
+  <si>
+    <t>The code just calls model generation, it is not explicitly tested.</t>
+  </si>
+  <si>
+    <t>tINITSpeedEval.m</t>
+  </si>
+  <si>
+    <t>preptINITModelHuman.m</t>
+  </si>
+  <si>
+    <t>Trivial script, no testing done.</t>
+  </si>
+  <si>
+    <t>Not tested, fairly trivial code, it just calls the model generation and measures time.</t>
+  </si>
+  <si>
+    <t>generate_PS_models.m</t>
+  </si>
+  <si>
+    <t>gen_PS_t68k.sh</t>
+  </si>
+  <si>
+    <t>gen_PS_hcat.sh</t>
+  </si>
+  <si>
+    <t>generate_PS_models_bulk.m</t>
+  </si>
+  <si>
+    <t>generate_PS_models_pseudobulk.m</t>
+  </si>
+  <si>
+    <t>AllTSNE.m</t>
+  </si>
+  <si>
+    <t>generate_LC3_CT_models.m</t>
+  </si>
+  <si>
+    <t>gen_gtex_ind.sh</t>
+  </si>
+  <si>
+    <t>generate_gtexind_models.m</t>
+  </si>
+  <si>
+    <t>generate_norm_models.m</t>
+  </si>
+  <si>
+    <t>run_quantile_eval.sh</t>
+  </si>
+  <si>
+    <t>run_tmm_eval.sh</t>
+  </si>
+  <si>
+    <t>generate_L4_models.m</t>
+  </si>
+  <si>
+    <t>genStructuralDataOldtINIT.m</t>
+  </si>
+  <si>
+    <t>The code is not tested, but is simple, and the results look reasonable.</t>
+  </si>
+  <si>
+    <t>generate_GTEx_models_old_tINIT.m</t>
+  </si>
+  <si>
+    <t>generate_GTEx_models_old_tINIT.sh</t>
+  </si>
+  <si>
+    <t>The TSNE is trivial, but the other logic is a bit complicated. There are no specific test cases, but  the code was tested thoroughly while it was written.</t>
+  </si>
+  <si>
+    <t>Trivial, not tested</t>
+  </si>
+  <si>
+    <t>extractTaskResults.m</t>
+  </si>
+  <si>
+    <t>getModelStructureData.m</t>
+  </si>
+  <si>
+    <t>Trivial function, just a few lines, not tested further.</t>
+  </si>
+  <si>
+    <t>run_mcor3_tasks_run_5.sh</t>
+  </si>
+  <si>
+    <t>TaskAnalysisMCOR3OnCluster.m</t>
+  </si>
+  <si>
+    <t>This code is fairly trivial, just calls other functions and merges data. No further testing was deemed needed</t>
+  </si>
+  <si>
+    <t>generate_MCOR3_bootstrap_models_run5.m</t>
+  </si>
+  <si>
+    <t>gen_mcor3_models_run_5.sh</t>
+  </si>
+  <si>
+    <t>run_lc3_tasks_run_5.sh</t>
+  </si>
+  <si>
+    <t>TaskAnalysisLC3OnCluster.m</t>
+  </si>
+  <si>
+    <t>gen_lc3_models_run_5.sh</t>
+  </si>
+  <si>
+    <t>generate_LC3_bootstrap_models_on_cluster.m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +409,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,9 +440,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +798,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -583,7 +828,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -594,7 +839,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -605,7 +850,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
@@ -616,45 +861,120 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
@@ -662,10 +982,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
@@ -673,10 +993,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
@@ -684,10 +1004,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
@@ -695,42 +1015,585 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>50</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>51</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" t="s">
+        <v>83</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B55" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60" t="s">
+        <v>83</v>
+      </c>
+      <c r="C60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B61" t="s">
+        <v>83</v>
+      </c>
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>93</v>
+      </c>
+      <c r="B62" t="s">
+        <v>105</v>
+      </c>
+      <c r="C62" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>94</v>
+      </c>
+      <c r="B63" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" t="s">
+        <v>83</v>
+      </c>
+      <c r="C64" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>95</v>
+      </c>
+      <c r="B65" t="s">
+        <v>65</v>
+      </c>
+      <c r="C65" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>97</v>
+      </c>
+      <c r="B66" t="s">
+        <v>83</v>
+      </c>
+      <c r="C66" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>98</v>
+      </c>
+      <c r="B68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>101</v>
+      </c>
+      <c r="B70" t="s">
+        <v>102</v>
+      </c>
+      <c r="C70" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>103</v>
+      </c>
+      <c r="B71" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>104</v>
+      </c>
+      <c r="B72" t="s">
+        <v>65</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B73" t="s">
+        <v>109</v>
+      </c>
+      <c r="C73" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>108</v>
+      </c>
+      <c r="B74" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>110</v>
+      </c>
+      <c r="B75" t="s">
+        <v>65</v>
+      </c>
+      <c r="C75" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>111</v>
+      </c>
+      <c r="B76" t="s">
+        <v>102</v>
+      </c>
+      <c r="C76" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>113</v>
+      </c>
+      <c r="B77" t="s">
+        <v>102</v>
+      </c>
+      <c r="C77" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>114</v>
+      </c>
+      <c r="B78" t="s">
+        <v>65</v>
+      </c>
+      <c r="C78" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>115</v>
+      </c>
+      <c r="B79" t="s">
+        <v>65</v>
+      </c>
+      <c r="C79" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>116</v>
+      </c>
+      <c r="B80" t="s">
+        <v>102</v>
+      </c>
+      <c r="C80" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B81" t="s">
+        <v>65</v>
+      </c>
+      <c r="C81" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>118</v>
+      </c>
+      <c r="B82" t="s">
+        <v>102</v>
+      </c>
+      <c r="C82" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified the code to use the implementation of ftINIT in RAVEN and to adapt to Human-GEM v. 1.12
</commit_message>
<xml_diff>
--- a/VerificationMatrix.xlsx
+++ b/VerificationMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\MatlabCode\projects\SingleCellModeling\SingleCellModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE450930-2DF5-4EC6-83D2-1D9F0FE74E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB9F01D-1005-4CBE-A814-A686D7167621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="99">
   <si>
     <t>File</t>
   </si>
@@ -150,63 +150,6 @@
     <t>TC 0104</t>
   </si>
   <si>
-    <t>checkTasksExt.m</t>
-  </si>
-  <si>
-    <t>fillGapsOpt.m</t>
-  </si>
-  <si>
-    <t>fitTasksOpt.m</t>
-  </si>
-  <si>
-    <t>getINITModel9.m</t>
-  </si>
-  <si>
-    <t>getMinNrFluxesOpt.m</t>
-  </si>
-  <si>
-    <t>groupRxnScores.m</t>
-  </si>
-  <si>
-    <t>runINIT9.m</t>
-  </si>
-  <si>
-    <t>prepINITModel.m</t>
-  </si>
-  <si>
-    <t>mergeLinear.m</t>
-  </si>
-  <si>
-    <t>rescaleModelForINIT.m</t>
-  </si>
-  <si>
-    <t>reverseRxns.m</t>
-  </si>
-  <si>
-    <t>T0003</t>
-  </si>
-  <si>
-    <t>T0004</t>
-  </si>
-  <si>
-    <t>T0001, T0002, T0050</t>
-  </si>
-  <si>
-    <t>T0001, T0002, T0003, T0050</t>
-  </si>
-  <si>
-    <t>T0001, T0002</t>
-  </si>
-  <si>
-    <t>T0006</t>
-  </si>
-  <si>
-    <t>T0007</t>
-  </si>
-  <si>
-    <t>This is a small change to an existing function in RAVEN. It has not been tested with test cases, although it has been manually tested to produce reasonable results.</t>
-  </si>
-  <si>
     <t>AnalyzeLC3.m</t>
   </si>
   <si>
@@ -249,12 +192,6 @@
     <t>prepMouseModel.m</t>
   </si>
   <si>
-    <t>getAATripletReactions.m</t>
-  </si>
-  <si>
-    <t>removeDrugReactions.m</t>
-  </si>
-  <si>
     <t>removeUnwantedReactions.m</t>
   </si>
   <si>
@@ -270,9 +207,6 @@
     <t>The code is fairly simple, not explicitly tested.</t>
   </si>
   <si>
-    <t>This code was tested while written, there are a few printouts commented out in the code.</t>
-  </si>
-  <si>
     <t>The code is trivial and not explicitly tested, although it was tested when written.</t>
   </si>
   <si>
@@ -391,6 +325,12 @@
   </si>
   <si>
     <t>generate_LC3_bootstrap_models_on_cluster.m</t>
+  </si>
+  <si>
+    <t>ftINIT</t>
+  </si>
+  <si>
+    <t>Tested by test cases in RAVEN - not explicitly traced here! The code in Human-GEM is fairly trivial and is not tested by test cases.</t>
   </si>
 </sst>
 </file>
@@ -725,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,32 +911,18 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
@@ -1004,10 +930,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
         <v>14</v>
@@ -1015,10 +941,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
         <v>14</v>
@@ -1026,10 +952,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
@@ -1037,10 +963,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -1048,10 +974,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
         <v>14</v>
@@ -1059,43 +985,43 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
         <v>48</v>
       </c>
-      <c r="B34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>112</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
         <v>14</v>
@@ -1103,10 +1029,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>47</v>
       </c>
       <c r="C37" t="s">
         <v>14</v>
@@ -1114,10 +1040,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C38" t="s">
         <v>14</v>
@@ -1125,10 +1051,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
@@ -1136,43 +1062,43 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41" t="s">
+    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>73</v>
+      <c r="A43" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
         <v>14</v>
@@ -1180,21 +1106,32 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C46" t="s">
         <v>14</v>
@@ -1202,10 +1139,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C47" t="s">
         <v>14</v>
@@ -1213,10 +1150,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" t="s">
         <v>61</v>
-      </c>
-      <c r="B48" t="s">
-        <v>67</v>
       </c>
       <c r="C48" t="s">
         <v>14</v>
@@ -1224,10 +1161,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C49" t="s">
         <v>14</v>
@@ -1235,10 +1172,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="C50" t="s">
         <v>14</v>
@@ -1246,10 +1183,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B51" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s">
         <v>14</v>
@@ -1260,40 +1197,40 @@
         <v>74</v>
       </c>
       <c r="B52" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C52" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C53" s="3" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C54" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>82</v>
+      <c r="A55" t="s">
+        <v>77</v>
       </c>
       <c r="B55" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
@@ -1301,10 +1238,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="C56" t="s">
         <v>14</v>
@@ -1312,10 +1249,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B57" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C57" t="s">
         <v>14</v>
@@ -1323,10 +1260,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C58" t="s">
         <v>14</v>
@@ -1334,10 +1271,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="C59" t="s">
         <v>14</v>
@@ -1345,10 +1282,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="C60" t="s">
         <v>14</v>
@@ -1356,10 +1293,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C61" t="s">
         <v>14</v>
@@ -1367,10 +1304,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B62" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C62" t="s">
         <v>14</v>
@@ -1378,10 +1315,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="C63" t="s">
         <v>14</v>
@@ -1389,10 +1326,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C64" t="s">
         <v>14</v>
@@ -1400,10 +1337,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C65" t="s">
         <v>14</v>
@@ -1411,10 +1348,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="C66" t="s">
         <v>14</v>
@@ -1422,10 +1359,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C67" t="s">
         <v>14</v>
@@ -1433,10 +1370,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B68" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C68" t="s">
         <v>14</v>
@@ -1444,10 +1381,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B69" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="C69" t="s">
         <v>14</v>
@@ -1455,144 +1392,12 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B70" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="C70" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>103</v>
-      </c>
-      <c r="B71" t="s">
-        <v>83</v>
-      </c>
-      <c r="C71" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>104</v>
-      </c>
-      <c r="B72" t="s">
-        <v>65</v>
-      </c>
-      <c r="C72" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>107</v>
-      </c>
-      <c r="B73" t="s">
-        <v>109</v>
-      </c>
-      <c r="C73" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>108</v>
-      </c>
-      <c r="B74" t="s">
-        <v>109</v>
-      </c>
-      <c r="C74" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>110</v>
-      </c>
-      <c r="B75" t="s">
-        <v>65</v>
-      </c>
-      <c r="C75" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>111</v>
-      </c>
-      <c r="B76" t="s">
-        <v>102</v>
-      </c>
-      <c r="C76" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>113</v>
-      </c>
-      <c r="B77" t="s">
-        <v>102</v>
-      </c>
-      <c r="C77" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>114</v>
-      </c>
-      <c r="B78" t="s">
-        <v>65</v>
-      </c>
-      <c r="C78" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>115</v>
-      </c>
-      <c r="B79" t="s">
-        <v>65</v>
-      </c>
-      <c r="C79" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>116</v>
-      </c>
-      <c r="B80" t="s">
-        <v>102</v>
-      </c>
-      <c r="C80" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>117</v>
-      </c>
-      <c r="B81" t="s">
-        <v>65</v>
-      </c>
-      <c r="C81" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>118</v>
-      </c>
-      <c r="B82" t="s">
-        <v>102</v>
-      </c>
-      <c r="C82" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Added code for plotting part of Fig. 5
</commit_message>
<xml_diff>
--- a/VerificationMatrix.xlsx
+++ b/VerificationMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\MatlabCode\projects\SingleCellModeling\SingleCellModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8B04C7-544A-4036-9DE3-9E6329A3F5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D67639E-1F70-42EE-8FB6-C2494A43A266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="110">
   <si>
     <t>File</t>
   </si>
@@ -355,6 +355,15 @@
   </si>
   <si>
     <t>A few small tests exist in the code, which was deemed sufficient.</t>
+  </si>
+  <si>
+    <t>gen_gtex_ind8.sh</t>
+  </si>
+  <si>
+    <t>generate_gtexind_models8.m</t>
+  </si>
+  <si>
+    <t>PlotMetAtlasTsne.R</t>
   </si>
 </sst>
 </file>
@@ -689,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,6 +830,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>105</v>
@@ -1119,23 +1136,23 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="B58" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="B60" t="s">
         <v>44</v>
@@ -1143,31 +1160,31 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B61" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B62" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B63" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
         <v>59</v>
@@ -1175,79 +1192,79 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B66" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B67" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B68" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B71" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B72" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B73" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B74" t="s">
         <v>44</v>
@@ -1255,7 +1272,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B75" t="s">
         <v>78</v>
@@ -1263,17 +1280,33 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>94</v>
+      </c>
+      <c r="B77" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>97</v>
+      </c>
+      <c r="B78" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>98</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B79" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the new functions to the verification matrix.
</commit_message>
<xml_diff>
--- a/VerificationMatrix.xlsx
+++ b/VerificationMatrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\MatlabCode\projects\SingleCellModeling\SingleCellModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D67639E-1F70-42EE-8FB6-C2494A43A266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DFC36A-B764-43B5-A026-ECBADC8C366E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="113">
   <si>
     <t>File</t>
   </si>
@@ -364,6 +364,15 @@
   </si>
   <si>
     <t>PlotMetAtlasTsne.R</t>
+  </si>
+  <si>
+    <t>listMetRxnsWithFluxes.m</t>
+  </si>
+  <si>
+    <t>This code was copied from another project - TME modeling, and works. No specific testing was deemed needed, the output looks very reasonable.</t>
+  </si>
+  <si>
+    <t>This code is fairly trivial, just calls other functions and merges data, as well as a simple task analysis. No further testing was deemed needed</t>
   </si>
 </sst>
 </file>
@@ -698,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +940,7 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1308,6 +1317,14 @@
       </c>
       <c r="B79" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>110</v>
+      </c>
+      <c r="B80" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates from revision 1. Some more updates will come.
</commit_message>
<xml_diff>
--- a/VerificationMatrix.xlsx
+++ b/VerificationMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\MatlabCode\projects\SingleCellModeling\SingleCellModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DFC36A-B764-43B5-A026-ECBADC8C366E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C45B88A-8C4C-42CB-A6B9-6DCB3B83CF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="122">
   <si>
     <t>File</t>
   </si>
@@ -373,6 +373,33 @@
   </si>
   <si>
     <t>This code is fairly trivial, just calls other functions and merges data, as well as a simple task analysis. No further testing was deemed needed</t>
+  </si>
+  <si>
+    <t>AssembleContData.m</t>
+  </si>
+  <si>
+    <t>getBootstrapJaccardData.m</t>
+  </si>
+  <si>
+    <t>This code is trivial and not tested.</t>
+  </si>
+  <si>
+    <t>Not tested more than that it can run and that it produces data with the right size. Not explicitly tested with test cases. The results look as expected though, so it most likely works.</t>
+  </si>
+  <si>
+    <t>generate_contamination_models.m</t>
+  </si>
+  <si>
+    <t>run_evaless_newalg2.sh</t>
+  </si>
+  <si>
+    <t>run_gen_contamination_models.sh</t>
+  </si>
+  <si>
+    <t>run_gen_depmap_models_newalg.sh</t>
+  </si>
+  <si>
+    <t>run_gen_depmap_models_newalg2.sh</t>
   </si>
 </sst>
 </file>
@@ -707,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,15 +980,15 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
         <v>54</v>
@@ -969,119 +996,111 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>46</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>82</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>58</v>
+      <c r="A48" t="s">
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>61</v>
-      </c>
-      <c r="B49" t="s">
-        <v>62</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
         <v>59</v>
@@ -1089,63 +1108,63 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="B52" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>67</v>
+      <c r="A53" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>68</v>
+      <c r="A54" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="B54" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>69</v>
+      <c r="A55" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>70</v>
+      <c r="A56" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
         <v>59</v>
@@ -1153,23 +1172,23 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B61" t="s">
         <v>59</v>
@@ -1177,23 +1196,23 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B64" t="s">
         <v>59</v>
@@ -1201,15 +1220,15 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B65" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B66" t="s">
         <v>59</v>
@@ -1217,7 +1236,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B67" t="s">
         <v>44</v>
@@ -1225,23 +1244,23 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="B68" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B69" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B70" t="s">
         <v>44</v>
@@ -1249,81 +1268,145 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B73" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B74" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B76" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B77" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B78" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B79" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>89</v>
+      </c>
+      <c r="B80" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>90</v>
+      </c>
+      <c r="B81" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>91</v>
+      </c>
+      <c r="B82" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>94</v>
+      </c>
+      <c r="B85" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>97</v>
+      </c>
+      <c r="B86" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>98</v>
+      </c>
+      <c r="B87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>110</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B88" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>